<commit_message>
+ 1 text from Azaev (1974)
</commit_message>
<xml_diff>
--- a/texts/azaev_text1.xlsx
+++ b/texts/azaev_text1.xlsx
@@ -31,469 +31,469 @@
     <t xml:space="preserve">russian</t>
   </si>
   <si>
-    <t xml:space="preserve">Цев г1олохъан гьек1ва вул1уда гьанила бета илала ета маг1ишати орсса.</t>
+    <t xml:space="preserve">Цев гIолохъан гьекIва вулIуда гьанила бета илала ета магIишати орсса.</t>
   </si>
   <si>
     <t xml:space="preserve">Однажды решил юноша отправиться на заработки, поискать счастья. Получил он благословения своей старушки-матери и пошел из родного села.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьек1уб дунелала вац1а ссакуйла ссаква маквасала гьанкъасала вагьу гьав вук1ида цеб инххи байлъи шамди гьарч1ч1ахи.</t>
+    <t xml:space="preserve">ГьекIуб дунелала вацIа ссакуйла ссаква маквасала гьанкъасала вагьу гьав вукIида цеб инххи байлъи шамди гьарчIчIахи.</t>
   </si>
   <si>
     <t xml:space="preserve">Долго шел он, но пришел в чужие края. Усталый и голодный присел он у речки отдохнуть. Напился он речной воды и задумался. Глянул на речку, а по ней яблоко плывет.</t>
   </si>
   <si>
-    <t xml:space="preserve">Лълъенила ххуду гъамдинала гуч1ада ургъалакьи гьарч1ч1ахик1оруди гьащуй гьагъида инххиди гьерда гъвалъа цеб инчу. Габ инчула бикку гьущуди инчулъи къамдуда.</t>
+    <t xml:space="preserve">Лълъенила ххуду гъамдинала гучIада ургъалакьи гьарчIчIахикIоруди гьащуй гьагъида инххиди гьерда гъвалъа цеб инчу. Габ инчула бикку гьущуди инчулъи къамдуда.</t>
   </si>
   <si>
     <t xml:space="preserve">Обрадовал­ся, выловил это яблоко юноша, тут же надкусил его.</t>
   </si>
   <si>
-    <t xml:space="preserve">Къамдамна мик1к1у борч1атада гьащуй рак1вара магъуда изну гуч1аб гьек1уб х1арам инчулъи цеб зук1к1у на мик1к1у маъир.</t>
+    <t xml:space="preserve">Къамдамна микIкIу борчIатада гьащуй ракIвара магъуда изну гучIаб гьекIуб хIарам инчулъи цеб зукIкIу на микIкIу маъир.</t>
   </si>
   <si>
     <t xml:space="preserve">И только про­глотил этот кусок, как вспомнил материнский наказ: -- Упаси тебя, Аллах, брать что-либо чужое без спросу.</t>
   </si>
   <si>
-    <t xml:space="preserve">Валла х1арам нала гъамду ден вук1и бегъевч1и ишкур гьаб инчулъи гъванек1вала квада вац1о гьущухи гьеру вул1италу хади буккик1абталу гьащуй рак1вара буккуда. Гьав гьалала гьирч1ч1у инщубда къай-матах1ла ибху гьаб инххи бикку гьала вел1уда. Гьав вук1ида инххи бикку гьала ваъала инщуй гоб инчу бижаб ахила мисик1аб эхха ахилъи гъванек1вала винсик1о талу.</t>
+    <t xml:space="preserve">Валла хIарам нала гъамду ден вукIи бегъевчIи ишкур гьаб инчулъи гъванекIвала квада вацIо гьущухи гьеру вулIиталу хади буккикIабталу гьащуй ракIвара буккуда. Гьав гьалала гьирчIчIу инщубда къай-матахIла ибху гьаб инххи бикку гьала велIуда. Гьав вукIида инххи бикку гьала ваъала инщуй гоб инчу бижаб ахила мисикIаб эхха ахилъи гъванекIвала винсикIо талу.</t>
   </si>
   <si>
     <t xml:space="preserve">Огорчился он своей забывчивости и решил пойти на поиски хозяина яблока, а, найдя его, попросить у него прощения.</t>
   </si>
   <si>
-    <t xml:space="preserve">Букьаб бидрикьи вел1уда гьав инххи бикку гьала эшта букьу бук1ала эшда макваса вук1ала инщубда ц1ц1инк1к1ив маъаб зук1к1уда г1умру цеб къамдаб инчу саъабу хъупи бештивч1абталу накварла руху.</t>
+    <t xml:space="preserve">Букьаб бидрикьи велIуда гьав инххи бикку гьала эшта букьу букIала эшда макваса вукIала инщубда цIцIинкIкIив маъаб зукIкIуда гIумру цеб къамдаб инчу саъабу хъупи бештивчIабталу накварла руху.</t>
   </si>
   <si>
     <t xml:space="preserve">Собрал он свои вещи и пошел вверх по течению речки, раз оттуда яблоко река принесла, там и сад и его хозяин быть должны, - решил юноша.</t>
   </si>
   <si>
-    <t xml:space="preserve">Цеб заман маъаруди гьав вац1ида цеб колилълъи муса.</t>
+    <t xml:space="preserve">Цеб заман маъаруди гьав вацIида цеб колилълъи муса.</t>
   </si>
   <si>
     <t xml:space="preserve">Очень жарким был день, но юноша шел вперед, хоть и мучил его голод невыносимо, а решил он дойти до цели, не становиться же ему, думал он, бесчестным из-за кусочка яблока взятого без спросу.</t>
   </si>
   <si>
-    <t xml:space="preserve">Коли бехъут1у хьваъабда ахила бук1ида ахикьи кьани бехъила бук1ида.</t>
+    <t xml:space="preserve">Коли бехъутIу хьваъабда ахила букIида ахикьи кьани бехъила букIида.</t>
   </si>
   <si>
     <t xml:space="preserve">Наконец он добрался до какого-то сада, через которого протекала речка.</t>
   </si>
   <si>
-    <t xml:space="preserve">Колилъи кагьуди гьина вел1аруди цев вахара гьек1ва винсида гьащуй релъи гьарч1ч1ахила вук1а. Гьув вахара гьек1ващуб микъассуб басала мигважула карчиццуб гьац1ахха бук1ида.</t>
+    <t xml:space="preserve">Колилъи кагьуди гьина велIаруди цев вахара гьекIва винсида гьащуй релъи гьарчIчIахила вукIа. Гьув вахара гьекIващуб микъассуб басала мигважула карчиццуб гьацIахха букIида.</t>
   </si>
   <si>
     <t xml:space="preserve">Подошел он к ограде, видит во дворе домик, а у домика дряхлый седой старик сидит.</t>
   </si>
   <si>
-    <t xml:space="preserve">Саламла икку гьав гьина гъваруди вахара адамиди гьащуб рела ибху гьикъари-бакъарила игьу гьав гьарч1ч1ахи вук1ода.</t>
+    <t xml:space="preserve">Саламла икку гьав гьина гъваруди вахара адамиди гьащуб рела ибху гьикъари-бакъарила игьу гьав гьарчIчIахи вукIода.</t>
   </si>
   <si>
     <t xml:space="preserve">Попросил юноша у старика разрешения войти к нему во двор, вошел и поздоровался. Ветви сада гнулись под тяжестью плодов. Обрадовался старик приходу гостя, взял его за руку, к дому повел.</t>
   </si>
   <si>
-    <t xml:space="preserve">Вахаращухи гьащуди мац1ц1уда габ инчу вахаращуб идаматалу.</t>
+    <t xml:space="preserve">Вахаращухи гьащуди мацIцIуда габ инчу вахаращуб идаматалу.</t>
   </si>
   <si>
     <t xml:space="preserve">-- Не ваше ли это, отец, яблоко? -- спросил юноша, показав ему надкушенный плод.</t>
   </si>
   <si>
-    <t xml:space="preserve">Вахаращуди мац1ц1уда дуй бат1алъи эбхула гьуб инчу лълъеб бук1ала талу.</t>
+    <t xml:space="preserve">Вахаращуди мацIцIуда дуй батIалъи эбхула гьуб инчу лълъеб букIала талу.</t>
   </si>
   <si>
     <t xml:space="preserve">-- И какая тебе разница чье оно? - удивилься старик.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьащуди масида вахаращухи т1оргуна.</t>
+    <t xml:space="preserve">Гьащуди масида вахаращухи тIоргуна.</t>
   </si>
   <si>
     <t xml:space="preserve">И тогда рассказал ему путник причину своих поисков.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гощуди жаваб иккуда гоб инчу инщуб гуч1и гьуб мисик1аб инщу воч1уха ваццуб талу.</t>
+    <t xml:space="preserve">Гощуди жаваб иккуда гоб инчу инщуб гучIи гьуб мисикIаб инщу вочIуха ваццуб талу.</t>
   </si>
   <si>
     <t xml:space="preserve">Старик ответил, что яблоко это не его, но возможно, что оно из сада его старшего брата, который живет чуть дальше от него.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьув воч1уха ваццила инххи бикку кванала гьала ваъала уду гьале вук1ир бич1ч1ода вахаращуди гьащуй. Гьал гулатак1оруди релъа гьав адамилъи гьарк1к1и гьуштуйта басала гьац1ц1аххаймалай адам гьингъида. Вахаращуй гьарк1к1уди гьав ил1ив нухлулавщухи вишадиталудала гьикьу гуч1и.</t>
+    <t xml:space="preserve">Гьув вочIуха ваццила инххи бикку кванала гьала ваъала уду гьале вукIир бичIчIода вахаращуди гьащуй. Гьал гулатакIоруди релъа гьав адамилъи гьаркIкIи гьуштуйта басала гьацIцIаххаймалай адам гьингъида. Вахаращуй гьаркIкIуди гьав илIив нухлулавщухи вишадиталудала гьикьу гучIи.</t>
   </si>
   <si>
     <t xml:space="preserve">Пока они шли к дому и говорили вышла из дому старушка, жена старика, такая же седая и дряхлая, как и он сам.</t>
   </si>
   <si>
-    <t xml:space="preserve">Вахаращуди маквала буху ц1ц1е инквамалаталу кьаруди инлъилъи рег1ел гуч1и талула гьикьу ишаххинду йаида гъургъала йагьу.</t>
+    <t xml:space="preserve">Вахаращуди маквала буху цIцIе инквамалаталу кьаруди инлъилъи регIел гучIи талула гьикьу ишаххинду йаида гъургъала йагьу.</t>
   </si>
   <si>
     <t xml:space="preserve">-- Покорми нашего гостя, -- попросил ее муж. -- Некогда мне с ним возиться! -- сказала старуха и ушла в дом что-то сердито ворча себе под нос.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьив макваса лъич1ик1улталула гьикьу гьав г1олохъан гьек1ва вахаращуб микъибит1ай рела ибху галълъа гьанкъеку орсса вул1уда. Гьенала бигьа игьу гьав инххи бикку гьала вел1уда.</t>
+    <t xml:space="preserve">Гьив макваса лъичIикIулталула гьикьу гьав гIолохъан гьекIва вахаращуб микъибитIай рела ибху галълъа гьанкъеку орсса вулIуда. Гьенала бигьа игьу гьав инххи бикку гьала велIуда.</t>
   </si>
   <si>
     <t xml:space="preserve">Поблагодарил путник старика, уверил его, что нисколько ни голоден, и пошел с трудом дальше.</t>
   </si>
   <si>
-    <t xml:space="preserve">Эшта ссаква вук1ала гьащуди микъи бухуда к1ейихоб колилъа.</t>
+    <t xml:space="preserve">Эшта ссаква вукIала гьащуди микъи бухуда кIейихоб колилъа.</t>
   </si>
   <si>
     <t xml:space="preserve">Вскоре добрался он до второго сада.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьалълъала винсида гьащуй гьуштуда гьек1ва релъи гьарч1ч1ахила вук1а амма гав гьек1ва квана гьикьи вук1ощуч1уку г1олохъан вук1ида. Гьащуб басала бекъин гьац1ахха бекъин беч1ер бук1ида.</t>
+    <t xml:space="preserve">Гьалълъала винсида гьащуй гьуштуда гьекIва релъи гьарчIчIахила вукIа амма гав гьекIва квана гьикьи вукIощучIуку гIолохъан вукIида. Гьащуб басала бекъин гьацIахха бекъин бечIер букIида.</t>
   </si>
   <si>
     <t xml:space="preserve">И здесь во дворе увидел он пожилого мужчину. Очень удивился юноша, когда узнал, что этот человек хоть и казался он намного моложе первого стари­ка, действительно доводился старшим братом.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьав мак1иди эб саъабу гьивда гащуха вуккидера масида.</t>
+    <t xml:space="preserve">Гьав макIиди эб саъабу гьивда гащуха вуккидера масида.</t>
   </si>
   <si>
     <t xml:space="preserve">Рассказал и ему юно­ша о причине своего прихода.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гащудила гьикьуда гоб инчу инщуб ахикьиссуб гуч1и гьуб миси букке инщу цевла воч1уха ваццубталу. Гав гьек1ващухила хъиду гьав мак1и вук1ида тамаша игьу. Ссе винсощуди гьикьу гьав гьек1ва инщу воч1уха вацциталу.</t>
+    <t xml:space="preserve">Гащудила гьикьуда гоб инчу инщуб ахикьиссуб гучIи гьуб миси букке инщу цевла вочIуха ваццубталу. Гав гьекIващухила хъиду гьав макIи вукIида тамаша игьу. Ссе винсощуди гьикьу гьав гьекIва инщу вочIуха вацциталу.</t>
   </si>
   <si>
     <t xml:space="preserve">Посмотрел на яблоко мужчина и ска­зал, что оно, видно, из сада его старшего брата, который живет еще дальше по реке.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьав воч1уха инлала вук1е гьащуч1у ссе гов хьваъабуда вахара вук1елълъи. Инщуй гьарк1к1и релъа гъаруди голъилъи гъванек1ващуди гьикьуда гьарк1к1ухи ц1ц1еруч1у ссе маквала бук1о ц1ц1е инкваймалаталу.</t>
+    <t xml:space="preserve">Гьав вочIуха инлала вукIе гьащучIу ссе гов хьваъабуда вахара вукIелълъи. Инщуй гьаркIкIи релъа гъаруди голъилъи гъванекIващуди гьикьуда гьаркIкIухи цIцIеручIу ссе маквала букIо цIцIе инкваймалаталу.</t>
   </si>
   <si>
     <t xml:space="preserve">Вышла из дому хозяйка, попросил ее муж накормить напоить гостя.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьассаг1атиталула гьикьу гащуй гьарк1к1и ишала йаъа ток1аб релъа йихху лъич1и.</t>
+    <t xml:space="preserve">ГьассагIатиталула гьикьу гащуй гьаркIкIи ишала йаъа токIаб релъа йихху лъичIи.</t>
   </si>
   <si>
     <t xml:space="preserve">-- Хорошо, сейчас, -- буркнула женщина и ушла в дом, да так и не показалась оттуда больше.</t>
   </si>
   <si>
-    <t xml:space="preserve">Галъилъи маква ссе гъидера гьирч1ч1у ч1арг1а гьенала ссе вел1уда.</t>
+    <t xml:space="preserve">Галъилъи маква ссе гъидера гьирчIчIу чIаргIа гьенала ссе велIуда.</t>
   </si>
   <si>
     <t xml:space="preserve">Надоело путнику ждать ее обеда, хоть голод томил его еще больше.</t>
   </si>
   <si>
-    <t xml:space="preserve">Иллаги-биллаги хадалидера гьав вац1ида гьабуйхоб колилъа.</t>
+    <t xml:space="preserve">Иллаги-биллаги хадалидера гьав вацIида гьабуйхоб колилъа.</t>
   </si>
   <si>
     <t xml:space="preserve">Поблагодарил пожилого человека и побрел дальше. Только к вечеру добрался измученный юноша до третьего сада и хутора в нем.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьав гьина вул1атада гьащуй данда гьингъва ида ригьуди чо вук1ада эрзаг1анда г1олохъан гьек1ва.</t>
+    <t xml:space="preserve">Гьав гьина вулIатада гьащуй данда гьингъва ида ригьуди чо вукIада эрзагIанда гIолохъан гьекIва.</t>
   </si>
   <si>
     <t xml:space="preserve">Как только он подошел к ограде, навстречу ему вышел человек в летах, но крепкий, бодрый и приветливый.</t>
   </si>
   <si>
-    <t xml:space="preserve">Басала гащуб къет1енигъва беч1ер бук1ида.</t>
+    <t xml:space="preserve">Басала гащуб къетIенигъва бечIер букIида.</t>
   </si>
   <si>
     <t xml:space="preserve">Ни сединки не было в его волосах, а с моложавого лица смотрели на путника веселые блестящие глаза.</t>
   </si>
   <si>
-    <t xml:space="preserve">Кьерила гащуб ч1иквар бук1ида.</t>
+    <t xml:space="preserve">Кьерила гащуб чIиквар букIида.</t>
   </si>
   <si>
     <t xml:space="preserve">И весь этот человек, хоть и загорел на солнце да и ветром был обветрен, показался юношетаким молодым по сравнению с первыми двумя, что юноша засомневался было, а туда ли он попал, куда надо было - к старшему брату тех двух?</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьущабда г1умрулъи йик1ида гащуй гьарк1к1ила.</t>
+    <t xml:space="preserve">Гьущабда гIумрулъи йикIида гащуй гьаркIкIила.</t>
   </si>
   <si>
     <t xml:space="preserve">Подошла и жена хозяина, такая же моложавая и приветливая, как и ее муж.</t>
   </si>
   <si>
-    <t xml:space="preserve">Вах1 гьав г1аламалъи эбхула гьеч1и воч1ухала вук1ихо гьабудала ваццуч1у вакьу гьашда гьолохъанч1у вагьихола вук1ихоталу рак1вара мугъуда ил1ивщуй.</t>
+    <t xml:space="preserve">ВахI гьав гIаламалъи эбхула гьечIи вочIухала вукIихо гьабудала ваццучIу вакьу гьашда гьолохъанчIу вагьихола вукIихоталу ракIвара мугъуда илIивщуй.</t>
   </si>
   <si>
     <t xml:space="preserve">Но на расспросы у юноши времени не было.</t>
   </si>
   <si>
-    <t xml:space="preserve">Колилъи гъванек1ващуди гьав ххеххо гьина инчида.</t>
+    <t xml:space="preserve">Колилъи гъванекIващуди гьав ххеххо гьина инчида.</t>
   </si>
   <si>
     <t xml:space="preserve">Повели его хозяе­ва в дом.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьащуй гъвани-ц1ек1а мучи муц1ц1ела т1асила бук1ода. Гьав вунча хъарду вул1идера гащу гьарк1к1уди маква х1адурода.</t>
+    <t xml:space="preserve">Гьащуй гъвани-цIекIа мучи муцIцIела тIасила букIода. Гьав вунча хъарду вулIидера гащу гьаркIкIуди маква хIадурода.</t>
   </si>
   <si>
     <t xml:space="preserve">Сразу же подала ему хозяйка умыться с дороги, помогла ему привести себя в порядок.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьав инкуй гьарч1ч1ахи вук1ода эбк1вала нала мац1ц1ич1ада энлъила гьавталула мац1ц1ич1ада.</t>
+    <t xml:space="preserve">Гьав инкуй гьарчIчIахи вукIода эбкIвала нала мацIцIичIада энлъила гьавталула мацIцIичIада.</t>
   </si>
   <si>
     <t xml:space="preserve">А пока он занимался этим и обед уж был для него подан, хоть никто еще не спросил кто он и откуда? Да зачем к ним в дом пожаловал?</t>
   </si>
   <si>
-    <t xml:space="preserve">Инква вул1аруди гъванек1ващуди гьурк1к1ухи гьикьуда ц1ц1еруй гъамди хъарпуз хваталу.</t>
+    <t xml:space="preserve">Инква вулIаруди гъванекIващуди гьуркIкIухи гьикьуда цIцIеруй гъамди хъарпуз хваталу.</t>
   </si>
   <si>
     <t xml:space="preserve">Когда они пообедали, хозяин попросил жену угостить гостя арбузом.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьарк1к1и хъарпузла ибху гьингъва ида. К1унт1уди габ хъарпузла квада ибху хъарпузалъила к1ват1адо гьикьуда габ хъарпуз гванзи гуч1и цебла хъарпуз хи буккик1абталу. Гьарк1к1уди цебла хъарпуз гьибгъвида. Гьенала кунт1уди гьарк1к1и йессухада йит1ода квана гванзи хъарпуз ибхи йаматалу. Гьена гъваб хъарпузла квада ибху гьикьуда гьабигье ищи бакъаб тайпа талу. Габ хъарпузла гъамду гьанкъулъи гъванек1ващуди гьав гъунду вигъода.</t>
+    <t xml:space="preserve">ГьаркIкIи хъарпузла ибху гьингъва ида. КIунтIуди габ хъарпузла квада ибху хъарпузалъила кIватIадо гьикьуда габ хъарпуз гванзи гучIи цебла хъарпуз хи буккикIабталу. ГьаркIкIуди цебла хъарпуз гьибгъвида. Гьенала кунтIуди гьаркIкIи йессухада йитIода квана гванзи хъарпуз ибхи йаматалу. Гьена гъваб хъарпузла квада ибху гьикьуда гьабигье ищи бакъаб тайпа талу. Габ хъарпузла гъамду гьанкъулъи гъванекIващуди гьав гъунду вигъода.</t>
   </si>
   <si>
     <t xml:space="preserve">Принесла она арбуз, взял его хозяин, похлопал по нему, прижал к уху, и отослал его с ней обратно, мол, не совсем удач­ный попался. Это повторилось несколько раз, пока хозяин, наконец, не похвалил принесенный женой арбуз.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьабуда зивди гьащуб адаб-хъулухъ игьуда эбк1вала нагъарда мац1ц1ич1ада.</t>
+    <t xml:space="preserve">Гьабуда зивди гьащуб адаб-хъулухъ игьуда эбкIвала нагъарда мацIцIичIада.</t>
   </si>
   <si>
     <t xml:space="preserve">Три дня прожил путник в доме этого садовника без забот и хлопот, отдохнул от дальнего пути в свое удовольствие.</t>
   </si>
   <si>
-    <t xml:space="preserve">Бугьуйхоб зивди мац1ц1уда гьащухи эбхула къвараб-бетам на игьи-бети нагъарда идама талу.</t>
+    <t xml:space="preserve">Бугьуйхоб зивди мацIцIуда гьащухи эбхула къвараб-бетам на игьи-бети нагъарда идама талу.</t>
   </si>
   <si>
     <t xml:space="preserve">И только на четвертый день спросил его хозяин: “Чем могу я тебе быть полезным, юноша? По какому делу ты сюда пожаловал?”</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьащуди масида т1оргу бул1аб нагъарла эб саъабив гьивда ага вуккидерала.</t>
+    <t xml:space="preserve">Гьащуди масида тIоргу булIаб нагъарла эб саъабив гьивда ага вуккидерала.</t>
   </si>
   <si>
     <t xml:space="preserve">Рассказал ему юноша о себе и о том, что с ним было.</t>
   </si>
   <si>
-    <t xml:space="preserve">Вахаращуй гьащуди инщуй да къамдам инчула гьагъо габ инчу дащуб ахикьиссуб идахуматалу мац1ц1уда.</t>
+    <t xml:space="preserve">Вахаращуй гьащуди инщуй да къамдам инчула гьагъо габ инчу дащуб ахикьиссуб идахуматалу мацIцIуда.</t>
   </si>
   <si>
     <t xml:space="preserve">Пока­зал надкушенное яблоко, спросил не из его ли оно сада.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьанкъулъи гъванек1ващуди гоб инчу инщуба ахикьиссуб бук1ир масида.</t>
+    <t xml:space="preserve">Гьанкъулъи гъванекIващуди гоб инчу инщуба ахикьиссуб букIир масида.</t>
   </si>
   <si>
     <t xml:space="preserve">Глянул садовник на яблоко и сказал, что оно из его сада.</t>
   </si>
   <si>
-    <t xml:space="preserve">Цеб квана рахъиди мак1ич1у ххунххулалхала хъиду мац1ц1уда гащуб ц1ц1ери эбхулаталу.</t>
+    <t xml:space="preserve">Цеб квана рахъиди макIичIу ххунххулалхала хъиду мацIцIуда гащуб цIцIери эбхулаталу.</t>
   </si>
   <si>
     <t xml:space="preserve">Потом он внимательно посмотрел в лицо юноше и спросил, как его зовут.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьащуди жаваб инкуда инщуб ц1ц1ери Х1абиб ида талу.</t>
+    <t xml:space="preserve">Гьащуди жаваб инкуда инщуб цIцIери ХIабиб ида талу.</t>
   </si>
   <si>
     <t xml:space="preserve">“Хабиб”, – ответил молодой человек. Глянул на него хозяин и снова о чем-то задумался.</t>
   </si>
   <si>
-    <t xml:space="preserve">Эхха бехут1уда гъвандола мац1ц1уда гав гьек1ва инщуч1у гьеру вул1уматалу.</t>
+    <t xml:space="preserve">Эхха бехутIуда гъвандола мацIцIуда гав гьекIва инщучIу гьеру вулIуматалу.</t>
   </si>
   <si>
     <t xml:space="preserve">-- Осмелюсь перебить твое раздумье, почтенный хозяин, и спрошу: “Простил ли ты мне за то, что взял я твое яблоко без спросу?”</t>
   </si>
   <si>
-    <t xml:space="preserve">Гав гьек1ващуди Х1абиби джаваб иккуда гьив гьеру вул1ик1о мин инщу йещи инчала талу. Эхха Х1абибиди джаваб ккидерада вигъич1ада гьикьуда гащуди инщуй йеши регъибалъила гуч1ай реъабалъила гуч1ай гьабдилъила боццу г1енкъила г1енкъи миц1ц1ила бегъихич1ай мак1идаталу.</t>
+    <t xml:space="preserve">Гав гьекIващуди ХIабиби джаваб иккуда гьив гьеру вулIикIо мин инщу йещи инчала талу. Эхха ХIабибиди джаваб ккидерада вигъичIада гьикьуда гащуди инщуй йеши регъибалъила гучIай реъабалъила гучIай гьабдилъила боццу гIенкъила гIенкъи мицIцIила бегъихичIай макIидаталу.</t>
   </si>
   <si>
     <t xml:space="preserve">-- Прошу, тебя юноша, но при одном условии: если женишься на моей дочери, -- сказал хозяин, и, не дожидаясь ответа юноши, поспешил ему сказать: "только знай, что у дочери моей ни рук, ни ног, и слепа она и глухонемая".</t>
   </si>
   <si>
-    <t xml:space="preserve">Виххич1ада бигьаигьу Х1абибиди джаваб иккуда гьив эбг1ала игьи разида мин гьеру вулълъабуссуб ва амма мац1ц1ич1ада хъизан игьи билълъивч1аб инщуй бегье мисала илухила мац1ц1у гъи вета гьивталу.</t>
+    <t xml:space="preserve">ВиххичIада бигьаигьу ХIабибиди джаваб иккуда гьив эбгIала игьи разида мин гьеру вулълъабуссуб ва амма мацIцIичIада хъизан игьи билълъивчIаб инщуй бегье мисала илухила мацIцIу гъи вета гьивталу.</t>
   </si>
   <si>
     <t xml:space="preserve">-- Я готов пойти на все, почтенный, -- спокойно ответил Хабиб. -- Лишь бы ты простил мне мою вину.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ваъи бегье минталула гьикьу гьащуди Х1абиб микъида вухуда гьанкъулъи гъванек1ващуди.</t>
+    <t xml:space="preserve">Ваъи бегье минталула гьикьу гьащуди ХIабиб микъида вухуда гьанкъулъи гъванекIващуди.</t>
   </si>
   <si>
     <t xml:space="preserve">Но, если дело касается женитьбы, я должен обязательно посоветоваться со своей матерью. А поэтому разреши мне хозяин, вернуться сначала домой, с ней все решить необходимо. Отпустил его садовник домой, проводя в дорогу.</t>
   </si>
   <si>
-    <t xml:space="preserve">Х1абиб ишхъа вац1ида. Гьащуди илухи бул1аб-бетам на масида. Илуди гьав гьулълъакуда вессуха вит1ода гьек1вала гьеку вул1айч1ада гьек1уб х1арам нала гъамду мин шихъа эпилъилаталу.</t>
+    <t xml:space="preserve">ХIабиб ишхъа вацIида. Гьащуди илухи булIаб-бетам на масида. Илуди гьав гьулълъакуда вессуха витIода гьекIвала гьеку вулIайчIада гьекIуб хIарам нала гъамду мин шихъа эпилъилаталу.</t>
   </si>
   <si>
     <t xml:space="preserve">Пришел Хабиб домой, рассказал матери обо всем, что с ним за время его отсутствия сталось.</t>
   </si>
   <si>
-    <t xml:space="preserve">Х1абиб инчулъи гъванек1ващуха вессухада вац1ида илулъи разулъирла масида.</t>
+    <t xml:space="preserve">ХIабиб инчулъи гъванекIващуха вессухада вацIида илулъи разулъирла масида.</t>
   </si>
   <si>
     <t xml:space="preserve">Мать его тут же послала назад, к садовнику. "Выполни все сынок, но исправь свою ошибку с яблоком." Вернулся Хабиб к хозяину яблока, сказал об одобрении ма­терью решении жениться на его дочери.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гъванек1ващуди бертини х1адурлъи гьи байбихьи игьуда.</t>
+    <t xml:space="preserve">ГъванекIващуди бертини хIадурлъи гьи байбихьи игьуда.</t>
   </si>
   <si>
     <t xml:space="preserve">Начал хозяин к свадьбе готовиться.</t>
   </si>
   <si>
-    <t xml:space="preserve">Амма Х1абиби т1ок1ам налъилъи ургъал бук1а гуч1и гьав гьек1ва гьеку вул1абуссуб. Ахареру бертин бук1и эгьел имакьурди Х1абибихи гьикьуда дуйда бах1арай гьагъила гьулъилъи магьари бигьи разилъир хила уда гьиунуссуб иша ваматалу.</t>
+    <t xml:space="preserve">Амма ХIабиби тIокIам налъилъи ургъал букIа гучIи гьав гьекIва гьеку вулIабуссуб. Ахареру бертин букIи эгьел имакьурди ХIабибихи гьикьуда дуйда бахIарай гьагъила гьулъилъи магьари бигьи разилъир хила уда гьиунуссуб иша ваматалу.</t>
   </si>
   <si>
     <t xml:space="preserve">Как-то незадолго до свадьбы сказал он юноше, что пора ему и с невестой познакомить­ся, да получить и у нее согласие выйти за него замуж. А когда Хабиб собрался уже идти к невесте предупредил его хозяин, что ни о каком прощении за яблоко и речи не может быть, если дочь его не согласится на брак, от того, что жених ей не понравится.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьулълъи мац1ц1ала джаваб ккима билълъе миц1ц1ила бегъихич1ай г1енкъи адамиталу рак1вара мугъуда Х1абиби.</t>
+    <t xml:space="preserve">Гьулълъи мацIцIала джаваб ккима билълъе мицIцIила бегъихичIай гIенкъи адамиталу ракIвара мугъуда ХIабиби.</t>
   </si>
   <si>
     <t xml:space="preserve">Удивился Хабиб заявлению, подумав: "Что толку в таких смотринах и знакомстве, если дочь садовника ни увидеть, ни услы­шать его не сможет."</t>
   </si>
   <si>
-    <t xml:space="preserve">Бук1алла имакьурич1у данда раша ссардай билълъич1ада гьав иша инщуйда йик1илъай гьарк1к1уха вел1уда. Иша вац1атада Х1абиб вихху веххуда.</t>
+    <t xml:space="preserve">БукIалла имакьуричIу данда раша ссардай билълъичIада гьав иша инщуйда йикIилъай гьаркIкIуха велIуда. Иша вацIатада ХIабиб вихху веххуда.</t>
   </si>
   <si>
     <t xml:space="preserve">Но ничего не сказал он отцу невесты и вошел в указанную ему комнату.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьащуй иши йинсида гьада хъиди баращхъай ч1иквар мак1и. Гаштуб ч1икварир гьащуй масатадала агьа гуч1и.</t>
+    <t xml:space="preserve">Гьащуй иши йинсида гьада хъиди баращхъай чIиквар макIи. Гаштуб чIикварир гьащуй масатадала агьа гучIи.</t>
   </si>
   <si>
     <t xml:space="preserve">А войдя туда, – глазам своим не поверил. Перед ним стояла совершенно здоровая девушка и такая красавица, какой он раньше и в мечтах своих представить не мог.</t>
   </si>
   <si>
-    <t xml:space="preserve">Галъилъи ч1иквар беч1ер гьабдилъихила къет1енгъва беч1ер бакьехила беххила кьимссирдехила гьайбатаб чергесаб лагихила ххунххулалъиссуб йешик1валъир мугъаб дангъвахила хъиду Х1абиб сапив веххуда.</t>
+    <t xml:space="preserve">Галъилъи чIиквар бечIер гьабдилъихила къетIенгъва бечIер бакьехила беххила кьимссирдехила гьайбатаб чергесаб лагихила ххунххулалъиссуб йешикIвалъир мугъаб дангъвахила хъиду ХIабиб сапив веххуда.</t>
   </si>
   <si>
     <t xml:space="preserve">Увидев онемевшего от удивления Хабиба, девушка встала и, улыбнувшись сказала ему: -- Нет, ты не ошибся, Хабиб, это та комната, куда тебе следовало войти, и я – твоя невеста.</t>
   </si>
   <si>
-    <t xml:space="preserve">Валла гьив мекъи вукку винсик1оталу рак1вара мугъу гьав цеквана вессхъа къиндуда. Гьащуй рак1вара мугъам на бич1ч1абцууб х1еренаб гьарч1ч1иди гьикьуда гьалълъиди мин т1ирдала мекъи вуккич1а ден ида дуй бах1арай талу.</t>
+    <t xml:space="preserve">Валла гьив мекъи вукку винсикIоталу ракIвара мугъу гьав цеквана вессхъа къиндуда. Гьащуй ракIвара мугъам на бичIчIабцууб хIеренаб гьарчIчIиди гьикьуда гьалълъиди мин тIирдала мекъи вуккичIа ден ида дуй бахIарай талу.</t>
   </si>
   <si>
     <t xml:space="preserve">И если раньше Хабиб не поверил своим глазам, то теперь он ушам своим не поверил. Дивно звучал для него ласковый голос девушки, любовался он ее стройным станом, струившимися по плечам длинными косами, нежным благородным лицом и газельими глазами, что смущенно смотрели на него из-под стрельчатых ресниц.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьай гьагъилада гьащуй гьай мак1ила идода гай мак1и Х1абибла идода.</t>
+    <t xml:space="preserve">Гьай гьагъилада гьащуй гьай макIила идода гай макIи ХIабибла идода.</t>
   </si>
   <si>
     <t xml:space="preserve">С пер­вого взгляда полюбил юноша красавицу. И девушка потом рассказала, что и она полюбила Хабиба сразу, как только увидела его во дворе.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гай мак1и ц1ц1ери зубаржати бук1ида. Галълъиди инлъилъида разилъир инкуда магьари бигьи.</t>
+    <t xml:space="preserve">Гай макIи цIцIери зубаржати букIида. Галълъиди инлъилъида разилъир инкуда магьари бигьи.</t>
   </si>
   <si>
     <t xml:space="preserve">Еще милее стал он ей, когда из рассказа отца узнала она о его честности, доброте и скромности.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ахареру бертинла игьу кутакаб зух1маткеп бук1ида.</t>
+    <t xml:space="preserve">Ахареру бертинла игьу кутакаб зухIматкеп букIида.</t>
   </si>
   <si>
     <t xml:space="preserve">На другой день и свадьбу сыграли, много радости и веселья было на этом свадебном пире.</t>
   </si>
   <si>
-    <t xml:space="preserve">Бертинла бул1у гьиволдалълъи мусек1оруди Х1абибиди имакьурхи мац1ц1уда инщуйда тамаша игьабугъа налъилъила бич1ч1ич1а беххвабугъа налъилъила х1акъалда.</t>
+    <t xml:space="preserve">Бертинла булIу гьиволдалълъи мусекIоруди ХIабибиди имакьурхи мацIцIуда инщуйда тамаша игьабугъа налъилъила бичIчIичIа беххвабугъа налъилъила хIакъалда.</t>
   </si>
   <si>
     <t xml:space="preserve">И лишь через несколько дней попросил Хабиб тестя расска­зать ему о своих братьях, объяснить, почему, он, самый старший из них, намного молохе их кажется. В чем тут секрет или волшеб­ство какое?</t>
   </si>
   <si>
-    <t xml:space="preserve">Имакьурди нусащухи т1оргу на масида.</t>
+    <t xml:space="preserve">Имакьурди нусащухи тIоргу на масида.</t>
   </si>
   <si>
     <t xml:space="preserve">-- Никакого волшебства тут нет, сын мой. А нашему секрету имя -- семейное счастье. И рассказал Хабибу тесть о братьях и о себе.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьеч1и ссе винсо вахара гьек1ва вук1ида гьеч1и зук1к1у вацци. Гьущуй гьарк1к1и сурай йиккурди г1умру питналъила маъа к1едала бекъа рахарода.</t>
+    <t xml:space="preserve">ГьечIи ссе винсо вахара гьекIва вукIида гьечIи зукIкIу вацци. Гьущуй гьаркIкIи сурай йиккурди гIумру питналъила маъа кIедала бекъа рахарода.</t>
   </si>
   <si>
     <t xml:space="preserve">Самому младшему брату довелась в жены на редкость злая и вздорная женщина.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьулълъа гьеххинду к1вах1аллъал заг1ипалла рул1уда.</t>
+    <t xml:space="preserve">Гьулълъа гьеххинду кIвахIаллъал загIипалла рулIуда.</t>
   </si>
   <si>
     <t xml:space="preserve">Не было у нее ни любви, ни уважения к нему.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьарк1к1иди кунт1уб адаб гьич1айда гьарк1к1уй къвараб кунт1уди гьич1айда питналъи г1умрула маъа рак1вала ч1агьич1а талих1ла бич1а реххула.</t>
+    <t xml:space="preserve">ГьаркIкIиди кунтIуб адаб гьичIайда гьаркIкIуй къвараб кунтIуди гьичIайда питналъи гIумрула маъа ракIвала чIагьичIа талихIла бичIа реххула.</t>
   </si>
   <si>
     <t xml:space="preserve">Да и он потом стал платить ей тем же. Вся жизнь проходит их в бес­конечных ссорах и скандалах.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьуб саъабу к1унт1уб баса карчи бул1у гьац1аххода.</t>
+    <t xml:space="preserve">Гьуб саъабу кIунтIуб баса карчи булIу гьацIаххода.</t>
   </si>
   <si>
     <t xml:space="preserve">Вот почему то так быстро они и со­старились, что не знали счастья и согласия, не было в их доме покоя и радости.</t>
   </si>
   <si>
-    <t xml:space="preserve">К1ейилъо ваццубла гьубда на бул1уда.</t>
+    <t xml:space="preserve">КIейилъо ваццубла гьубда на булIуда.</t>
   </si>
   <si>
     <t xml:space="preserve">И среднему брату, тоже с женитьбой не повезло.</t>
   </si>
   <si>
-    <t xml:space="preserve">Бук1ала гьущуй гьарк1к1и квана мадарай маг1ишати хьваъай йик1ирди гьал квана мадаралда реххуда. Гьулардугъалу гьущуб баса бекъинуч1а гьац1аххайч1ада.</t>
+    <t xml:space="preserve">БукIала гьущуй гьаркIкIи квана мадарай магIишати хьваъай йикIирди гьал квана мадаралда реххуда. Гьулардугъалу гьущуб баса бекъинучIа гьацIаххайчIада.</t>
   </si>
   <si>
     <t xml:space="preserve">Но все же чуть помягче характером у него жена. Хоть и жизнь в его доме на­много легче, чем в семье младшего брата слохилась, но наложила она такой тяжелой печати на него и жену.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьащу имакьур гьеч1и воч1уха вацци вук1ида. Гьащуй гьарк1к1и хьваъай йиккуда.</t>
+    <t xml:space="preserve">Гьащу имакьур гьечIи вочIуха вацци вукIида. Гьащуй гьаркIкIи хьваъай йиккуда.</t>
   </si>
   <si>
     <t xml:space="preserve">По иному сложилось все в семье тестя Хабиба.</t>
   </si>
   <si>
-    <t xml:space="preserve">Целуб целухахоб ххиралъирдила целуди игьаб адабидирдила гьалуб г1умру реццихху талих1алъи маъида.</t>
+    <t xml:space="preserve">Целуб целухахоб ххиралъирдила целуди игьаб адабидирдила гьалуб гIумру реццихху талихIалъи маъида.</t>
   </si>
   <si>
     <t xml:space="preserve">Они с женой любили и уважали друг друга, берегли один другого от беды и огорчений, добрая и милая жена во всем мужу и помощница и опора. Счастливо прожили они много лет и теперь в их доме всегда мир и согласие царят.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьулардугъалу гьал рахарайч1ада реххуда.</t>
+    <t xml:space="preserve">Гьулардугъалу гьал рахарайчIада реххуда.</t>
   </si>
   <si>
     <t xml:space="preserve">Вот и не растратили они своих сил и здоровья, не состарились преждевременно.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьеч1и воч1уха ваццуй гьеч1и ургъаллълъи на бук1ида йешилълъи къадрав кунт1амахи вуккик1оталу.</t>
+    <t xml:space="preserve">ГьечIи вочIуха ваццуй гьечIи ургъаллълъи на букIида йешилълъи къадрав кунтIамахи вуккикIоталу.</t>
   </si>
   <si>
     <t xml:space="preserve">И единственной заботой тестя рань­ше было желание уберечь свою единственную дочь от несчастного брака с жестоким, злым человеком.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьулардугъалу эштуб раша гье гъвала гьащуди йеши икку гуч1и лълъек1вала.</t>
+    <t xml:space="preserve">Гьулардугъалу эштуб раша гье гъвала гьащуди йеши икку гучIи лълъекIвала.</t>
   </si>
   <si>
     <t xml:space="preserve">Уже не раз отказывал он жени­хам, потому что ни один из них не пришелся дочери по сердцу.</t>
   </si>
   <si>
-    <t xml:space="preserve">Къамдам лълъедик1вала ургъал гьихич1аб инххиди гьерда бел1а мисаб инчу къамду маъир саъабу дунелла ссарду гьуб инчулъи гъванек1ва гьеру вул1айталу гье гъо гьек1ва йах1лълъи гванзи кунт1ек1ва винсик1оталу рак1варала мугъу вул1уда зубаржатилъи има гье гъо ц1ц1еруб х1ал ххинц1ц1ай.</t>
+    <t xml:space="preserve">Къамдам лълъедикIвала ургъал гьихичIаб инххиди гьерда белIа мисаб инчу къамду маъир саъабу дунелла ссарду гьуб инчулъи гъванекIва гьеру вулIайталу гье гъо гьекIва йахIлълъи гванзи кунтIекIва винсикIоталу ракIварала мугъу вулIуда зубаржатилъи има гье гъо цIцIеруб хIал ххинцIцIай.</t>
   </si>
   <si>
     <t xml:space="preserve">И еще вот о чем сказал своему зятю садовник. Когда Хабиб пришел к ним издалека только за тем, чтобы попросить прощения лишь за откушанное яблоко, первое о чем подумал он - это о честности и порядочности юноши.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьулардугъалу гьикьуда гащуди Х1абибихи инщуй ч1икварла гуч1ай бешеналълъу йеххвай, сурухъай йеши инча талу.</t>
+    <t xml:space="preserve">Гьулардугъалу гьикьуда гащуди ХIабибихи инщуй чIикварла гучIай бешеналълъу йеххвай, сурухъай йеши инча талу.</t>
   </si>
   <si>
     <t xml:space="preserve">А пока отдыхал Хабиб у них в доме после дальней дороги, садовник окончательно убедился в том, что это добрый человек, которому и судьбу дочери вручить не страшно.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьу гьинц1ц1иц1ц1ида йах1илълъи х1алимав кунт1ек1ва винсала гьущуб рак1ва гурх1и букке бешеналълъу йеххвай талих1 бич1ай мак1и гьуй инчила рази вукке гьу ва гьулада нагагьалдассан гьушутуй мак1и инчи гьу гьена разала гьущуди гьиц1ц1иц1ц1ида гьубда къайдади бешеналълъу йеххвала гьуй орссала йилавч1айталу рак1вара мугъуда имуй.</t>
+    <t xml:space="preserve">Гьу гьинцIцIицIцIида йахIилълъи хIалимав кунтIекIва винсала гьущуб ракIва гурхIи букке бешеналълъу йеххвай талихI бичIай макIи гьуй инчила рази вукке гьу ва гьулада нагагьалдассан гьушутуй макIи инчи гьу гьена разала гьущуди гьицIцIицIцIида гьубда къайдади бешеналълъу йеххвала гьуй орссала йилавчIайталу ракIвара мугъуда имуй.</t>
   </si>
   <si>
     <t xml:space="preserve">А чтобы испытать его окончательно он и выдумал историю об урод­стве своей дочери: уж если из долга возьмет такую в жены человек, то не оставит он своей жены, если с ней и действительно несчастье случится.</t>
   </si>
   <si>
-    <t xml:space="preserve">Имуй бат1ада идода илухи мац1ц1ич1ада регьина Х1абиб вул1ич1ир ва гьулада илухи мац1ц1игъалу ишхъа вац1ц1идера к1вах1алич1ада гьу ваъир.</t>
+    <t xml:space="preserve">Имуй батIада идода илухи мацIцIичIада регьина ХIабиб вулIичIир ва гьулада илухи мацIцIигъалу ишхъа вацIцIидера кIвахIаличIада гьу ваъир.</t>
   </si>
   <si>
     <t xml:space="preserve">Еще больше понравился Хабиб будущему тестю, когда он попросил отпустить его домой, чтобы посоветоваться с матерью о женитьбе, взять ее согласие.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьуб налълъиеку имуй бич1ч1уда Х1абиб йешилуб адаб гьиххо вах1ишийаб г1амал гуч1о гьек1ва вук1ир. Илуб адаб гьихо илухи гьант1ук1а риккихо гьек1ващуди цела йешилубла адаб билайхич1аб бук1ири мук1урав гьек1ва вук1ида има.</t>
+    <t xml:space="preserve">Гьуб налълъиеку имуй бичIчIуда ХIабиб йешилуб адаб гьиххо вахIишийаб гIамал гучIо гьекIва вукIир. Илуб адаб гьихо илухи гьантIукIа риккихо гьекIващуди цела йешилубла адаб билайхичIаб букIири мукIурав гьекIва вукIида има.</t>
   </si>
   <si>
     <t xml:space="preserve">Тот, кто с родной матерью считает­ся, тот уважит и мать своих детей, – жену свою, -- подумал тогда садовник.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьеч1и бессхъе т1оргу на бакъаб къайдалъа гъваруди ва гьулада Х1абиб гьащуб рак1ва разийав гьек1ва винсаруди имуди гьивда Х1абиб вешта ида йешилълъихи мац1ц1и ва гьулада йешилълъи гьу идайк1омахиталу ешилълъи рак1ва къварам на бул1ич1а бук1игъалу. Йешилъи къоро бук1ир бич1ч1арудич1а имуди магьари бигьу гуч1и.</t>
+    <t xml:space="preserve">ГьечIи бессхъе тIоргу на бакъаб къайдалъа гъваруди ва гьулада ХIабиб гьащуб ракIва разийав гьекIва винсаруди имуди гьивда ХIабиб вешта ида йешилълъихи мацIцIи ва гьулада йешилълъи гьу идайкIомахиталу ешилълъи ракIва къварам на булIичIа букIигъалу. Йешилъи къоро букIир бичIчIарудичIа имуди магьари бигьу гучIи.</t>
   </si>
   <si>
     <t xml:space="preserve">Уверившись в добропорядочности Хабиба, позволил он ему встретиться с дочерью, чтобы и ее чувства испытать.</t>
   </si>
   <si>
-    <t xml:space="preserve">Гьеч1и бессехъе гьаб т1оргу на маса бул1аруди имуди гьикьуда нусащухи гьеч1и къварихам на г1умурулъи гьину регьинлъи талих1хулк1улталу.</t>
+    <t xml:space="preserve">ГьечIи бессехъе гьаб тIоргу на маса булIаруди имуди гьикьуда нусащухи гьечIи къварихам на гIумурулъи гьину регьинлъи талихIхулкIулталу.</t>
   </si>
   <si>
     <t xml:space="preserve">-- Помни, сын мой, самое главное в жизни -- семейное счастье, заключил свой рассказ тесть Хабиба.</t>
@@ -599,8 +599,8 @@
   </sheetPr>
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B82" activeCellId="0" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>